<commit_message>
Updates to Negative Jump Algorithm documents
</commit_message>
<xml_diff>
--- a/Documents/USNO Tai - UTC 2.xlsx
+++ b/Documents/USNO Tai - UTC 2.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jay\Documents\Ultimate Datetime Datatype\Ultimate Datetime\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80920F-4097-4EF6-A42F-C01B34796A0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="19440" windowHeight="10035"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>1.4228180 S + (MJD - 37300.) X 0.001296 S</t>
   </si>
@@ -148,12 +162,6 @@
     <t>The green rows represent forward jumps in TAI time.  Specifically, at the start of an interval represented by a green row, the TAI time jumps when viewed from the prospective of the UTC time.  Any TAI time within that range will be converted to the same UTC time.</t>
   </si>
   <si>
-    <t>The yellow rows represent backward jumps in TAI time.  As a result, every TAI time within the range corresponds to 2, distinct UTC times.  To handle this properly, we need to associate a before or after flag with the TAI time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    This can be done the same way a sign was added to relative TAI time.</t>
-  </si>
-  <si>
     <t>23:59:59.95</t>
   </si>
   <si>
@@ -176,17 +184,20 @@
   </si>
   <si>
     <t>00:00:06.285682003</t>
+  </si>
+  <si>
+    <t>The yellow rows represent backward jumps in TAI time.  As a result, every TAI time within the range corresponds to 2, distinct UTC times.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
     <numFmt numFmtId="165" formatCode="0.000000000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -565,6 +576,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -857,40 +871,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="6" customWidth="1"/>
     <col min="6" max="6" width="32" style="27" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="5" customWidth="1"/>
     <col min="8" max="8" width="30" style="6" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="15.40625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.86328125" style="6" customWidth="1"/>
     <col min="11" max="11" width="43" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.86328125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="12.1328125" style="6" customWidth="1"/>
     <col min="17" max="17" width="23" style="6" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="6" customWidth="1"/>
-    <col min="19" max="21" width="9.140625" style="6"/>
-    <col min="22" max="22" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="9.140625" style="6"/>
-    <col min="25" max="16384" width="9.140625" style="7"/>
+    <col min="18" max="18" width="10.86328125" style="6" customWidth="1"/>
+    <col min="19" max="21" width="9.1328125" style="6"/>
+    <col min="22" max="22" width="16.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9.1328125" style="6"/>
+    <col min="25" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="10" customFormat="1">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="15"/>
@@ -916,7 +930,7 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
     </row>
-    <row r="2" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="10" customFormat="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="15"/>
@@ -948,7 +962,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="10" customFormat="1">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1002,7 +1016,7 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
     </row>
-    <row r="4" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="10" customFormat="1">
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
@@ -1064,7 +1078,7 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" customFormat="1">
       <c r="A5" s="2">
         <v>22282</v>
       </c>
@@ -1075,7 +1089,7 @@
         <v>22493</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2">
         <f>A5</f>
@@ -1089,7 +1103,7 @@
         <v>22494</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5">
         <f>A5+2415018.5</f>
@@ -1124,31 +1138,31 @@
         <v>1.6975699999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="25" customFormat="1">
       <c r="A6" s="21">
         <v>22493</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="22">
         <v>22494</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="21">
         <v>22494</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G6" s="22">
         <f>E6</f>
         <v>22494</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
@@ -1157,12 +1171,12 @@
       <c r="M6" s="24"/>
       <c r="N6" s="24"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" s="5">
         <v>22494</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="5">
         <f>A8</f>
@@ -1175,7 +1189,7 @@
         <v>22494</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G7" s="13">
         <f>C7</f>
@@ -1222,7 +1236,7 @@
         <v>-4.9999999999999822E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24">
       <c r="A8" s="5">
         <v>22647</v>
       </c>
@@ -1288,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="20" customFormat="1">
       <c r="A9" s="16">
         <f>C8</f>
         <v>23316</v>
@@ -1327,7 +1341,7 @@
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24">
       <c r="A10" s="5">
         <v>23316</v>
       </c>
@@ -1394,7 +1408,7 @@
         <v>0.10000000000000053</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24">
       <c r="A11" s="5">
         <v>23377</v>
       </c>
@@ -1461,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" s="20" customFormat="1">
       <c r="A12" s="16">
         <f>C11</f>
         <v>23468</v>
@@ -1500,7 +1514,7 @@
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24">
       <c r="A13" s="5">
         <v>23468</v>
       </c>
@@ -1567,7 +1581,7 @@
         <v>9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" s="20" customFormat="1">
       <c r="A14" s="16">
         <f>C13</f>
         <v>23621</v>
@@ -1606,7 +1620,7 @@
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24">
       <c r="A15" s="5">
         <v>23621</v>
       </c>
@@ -1673,7 +1687,7 @@
         <v>0.10000000000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" s="20" customFormat="1">
       <c r="A16" s="16">
         <f>C15</f>
         <v>23743</v>
@@ -1712,7 +1726,7 @@
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18">
       <c r="A17" s="5">
         <v>23743</v>
       </c>
@@ -1779,7 +1793,7 @@
         <v>0.10000000000000009</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" s="20" customFormat="1">
       <c r="A18" s="16">
         <f>C17</f>
         <v>23802</v>
@@ -1818,7 +1832,7 @@
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18">
       <c r="A19" s="5">
         <v>23802</v>
       </c>
@@ -1885,7 +1899,7 @@
         <v>0.10000000000000009</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="20" customFormat="1">
       <c r="A20" s="16">
         <f>C19</f>
         <v>23924</v>
@@ -1922,7 +1936,7 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18">
       <c r="A21" s="5">
         <v>23924</v>
       </c>
@@ -1989,7 +2003,7 @@
         <v>0.10000000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="20" customFormat="1">
       <c r="A22" s="16">
         <f>C21</f>
         <v>23986</v>
@@ -2028,7 +2042,7 @@
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18">
       <c r="A23" s="5">
         <v>23986</v>
       </c>
@@ -2095,7 +2109,7 @@
         <v>9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18">
       <c r="A24" s="5">
         <v>24108</v>
       </c>
@@ -2106,7 +2120,7 @@
         <v>24868</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5">
         <f>A24</f>
@@ -2117,11 +2131,10 @@
         <v>00:00:04.3131700</v>
       </c>
       <c r="G24" s="13">
-        <f>C24</f>
-        <v>24868</v>
+        <v>24869</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" si="0"/>
@@ -2160,32 +2173,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" s="25" customFormat="1">
       <c r="A25" s="21">
         <v>24868</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="21">
         <v>24869</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="21">
         <f>G24</f>
-        <v>24868</v>
+        <v>24869</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G25" s="22">
         <f>E25</f>
-        <v>24868</v>
+        <v>24869</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
@@ -2194,12 +2207,12 @@
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18">
       <c r="A26" s="5">
         <v>24869</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5">
         <f>A28</f>
@@ -2209,10 +2222,10 @@
         <v>30</v>
       </c>
       <c r="E26" s="5">
-        <v>22494</v>
+        <v>24869</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G26" s="13">
         <f>C26</f>
@@ -2259,7 +2272,7 @@
         <v>-0.10000000000000053</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" s="20" customFormat="1">
       <c r="A27" s="16">
         <f>C26</f>
         <v>26299</v>
@@ -2298,7 +2311,7 @@
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18">
       <c r="A28" s="5">
         <v>26299</v>
       </c>
@@ -2332,26 +2345,26 @@
         <v>0.10775800000000046</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18">
       <c r="H30" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K30" s="32">
         <f>1.69757000075 - 1.64756999925</f>
         <v>5.0000001500000169E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18">
       <c r="H31" s="31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="6" t="s">
         <v>40</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K32" s="6">
         <f>6.285682003 - 6.185681997</f>
@@ -2362,36 +2375,31 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
         <v>41</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L33" s="33">
         <f>1.422818 + (212-0.05/86400)*0.001296</f>
         <v>1.69756999925</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>